<commit_message>
Added output.xls folders for sa and hc
</commit_message>
<xml_diff>
--- a/SA/output.xlsx
+++ b/SA/output.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ackley" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="griewank" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="schwefel" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="rastrigin" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="sphere" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="rotatedhyperellipsoid" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="perm" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="zakharov" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="rosenbrock" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="damavandi" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ackley" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="griewank" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="schwefel" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rastrigin" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sphere" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rotatedhyperellipsoid" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="perm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="zakharov" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rosenbrock" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="damavandi" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -508,13 +508,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.1378950216650342</v>
+        <v>0.07596752595681984</v>
       </c>
       <c r="H2" t="n">
-        <v>21.69408</v>
+        <v>21.7929</v>
       </c>
       <c r="I2" t="n">
-        <v>21.5672</v>
+        <v>21.7227</v>
       </c>
     </row>
     <row r="3">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.05335000468603907</v>
+        <v>0.09212023664754337</v>
       </c>
       <c r="H3" t="n">
-        <v>21.74026</v>
+        <v>21.71274</v>
       </c>
       <c r="I3" t="n">
-        <v>21.6843</v>
+        <v>21.5946</v>
       </c>
     </row>
     <row r="4">
@@ -574,13 +574,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.09707005202429936</v>
+        <v>0.1586123355858529</v>
       </c>
       <c r="H4" t="n">
-        <v>21.7304</v>
+        <v>21.72526</v>
       </c>
       <c r="I4" t="n">
-        <v>21.6173</v>
+        <v>21.5619</v>
       </c>
     </row>
     <row r="5">
@@ -607,13 +607,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.1850059917948605</v>
+        <v>0.1533800345546995</v>
       </c>
       <c r="H5" t="n">
-        <v>21.69168</v>
+        <v>21.7266</v>
       </c>
       <c r="I5" t="n">
-        <v>21.3909</v>
+        <v>21.4952</v>
       </c>
     </row>
     <row r="6">
@@ -640,13 +640,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.140337030038401</v>
+        <v>0.08188291641119327</v>
       </c>
       <c r="H6" t="n">
-        <v>21.67188</v>
+        <v>21.80532</v>
       </c>
       <c r="I6" t="n">
-        <v>21.5186</v>
+        <v>21.7122</v>
       </c>
     </row>
     <row r="7">
@@ -673,13 +673,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.09240426397087763</v>
+        <v>0.1116575702762732</v>
       </c>
       <c r="H7" t="n">
-        <v>21.68424</v>
+        <v>21.71374</v>
       </c>
       <c r="I7" t="n">
-        <v>21.5358</v>
+        <v>21.5609</v>
       </c>
     </row>
   </sheetData>
@@ -767,13 +767,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>24.13625500470195</v>
+        <v>17.93712769196897</v>
       </c>
       <c r="H2" t="n">
-        <v>55.79652</v>
+        <v>39.76456</v>
       </c>
       <c r="I2" t="n">
-        <v>23.4379</v>
+        <v>16.018</v>
       </c>
     </row>
     <row r="3">
@@ -800,13 +800,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>30.54951424878962</v>
+        <v>20.85593328539867</v>
       </c>
       <c r="H3" t="n">
-        <v>54.00298</v>
+        <v>53.2081</v>
       </c>
       <c r="I3" t="n">
-        <v>27.8209</v>
+        <v>19.8783</v>
       </c>
     </row>
     <row r="4">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>16.24764600079039</v>
+        <v>28.90766451052385</v>
       </c>
       <c r="H4" t="n">
-        <v>51.83572</v>
+        <v>31.61004</v>
       </c>
       <c r="I4" t="n">
-        <v>31.3822</v>
+        <v>7.9318</v>
       </c>
     </row>
     <row r="5">
@@ -866,13 +866,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5.199196474745014</v>
+        <v>37.82769697582712</v>
       </c>
       <c r="H5" t="n">
-        <v>11.60244</v>
+        <v>55.25259999999999</v>
       </c>
       <c r="I5" t="n">
-        <v>8.4856</v>
+        <v>4.4936</v>
       </c>
     </row>
     <row r="6">
@@ -899,13 +899,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>50.1512823319803</v>
+        <v>30.24290975291564</v>
       </c>
       <c r="H6" t="n">
-        <v>54.08632</v>
+        <v>48.01456</v>
       </c>
       <c r="I6" t="n">
-        <v>3.6811</v>
+        <v>18.1499</v>
       </c>
     </row>
     <row r="7">
@@ -932,13 +932,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>48.60243915530371</v>
+        <v>21.1288959196878</v>
       </c>
       <c r="H7" t="n">
-        <v>52.7437</v>
+        <v>33.0321</v>
       </c>
       <c r="I7" t="n">
-        <v>14.5523</v>
+        <v>3.5803</v>
       </c>
     </row>
   </sheetData>
@@ -1026,13 +1026,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>146.6541135970212</v>
+        <v>87.92449984035734</v>
       </c>
       <c r="H2" t="n">
-        <v>764.78314</v>
+        <v>1022.16538</v>
       </c>
       <c r="I2" t="n">
-        <v>511.8755</v>
+        <v>883.2292</v>
       </c>
     </row>
     <row r="3">
@@ -1059,13 +1059,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>181.5509886698554</v>
+        <v>140.9240395389055</v>
       </c>
       <c r="H3" t="n">
-        <v>1031.99658</v>
+        <v>917.2071600000002</v>
       </c>
       <c r="I3" t="n">
-        <v>747.715</v>
+        <v>727.1133</v>
       </c>
     </row>
     <row r="4">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>72.77470724927025</v>
+        <v>104.6777782946313</v>
       </c>
       <c r="H4" t="n">
-        <v>840.5432199999999</v>
+        <v>901.1131000000001</v>
       </c>
       <c r="I4" t="n">
-        <v>746.9195</v>
+        <v>785.1153</v>
       </c>
     </row>
     <row r="5">
@@ -1125,13 +1125,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>78.61355711594524</v>
+        <v>102.8395656484654</v>
       </c>
       <c r="H5" t="n">
-        <v>912.92232</v>
+        <v>961.5845999999999</v>
       </c>
       <c r="I5" t="n">
-        <v>825.1355</v>
+        <v>858.9081</v>
       </c>
     </row>
     <row r="6">
@@ -1158,13 +1158,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>218.0418751825277</v>
+        <v>142.2109641956029</v>
       </c>
       <c r="H6" t="n">
-        <v>893.5845400000001</v>
+        <v>990.3490400000001</v>
       </c>
       <c r="I6" t="n">
-        <v>617.2782</v>
+        <v>871.9924</v>
       </c>
     </row>
     <row r="7">
@@ -1191,13 +1191,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>183.9481399840372</v>
+        <v>284.0696350939763</v>
       </c>
       <c r="H7" t="n">
-        <v>920.5381199999999</v>
+        <v>781.6322</v>
       </c>
       <c r="I7" t="n">
-        <v>794.5713</v>
+        <v>433.283</v>
       </c>
     </row>
   </sheetData>
@@ -1285,13 +1285,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1298.474306205663</v>
+        <v>877.1541750300074</v>
       </c>
       <c r="H2" t="n">
-        <v>12686.29762</v>
+        <v>13128.63494</v>
       </c>
       <c r="I2" t="n">
-        <v>11135.8517</v>
+        <v>12256.6829</v>
       </c>
     </row>
     <row r="3">
@@ -1318,13 +1318,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1238.650823175695</v>
+        <v>1320.17973868919</v>
       </c>
       <c r="H3" t="n">
-        <v>12154.27968</v>
+        <v>12040.1156</v>
       </c>
       <c r="I3" t="n">
-        <v>10666.37</v>
+        <v>10945.053</v>
       </c>
     </row>
     <row r="4">
@@ -1351,13 +1351,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>717.2496831159874</v>
+        <v>481.083244658903</v>
       </c>
       <c r="H4" t="n">
-        <v>12633.85004</v>
+        <v>12678.81668</v>
       </c>
       <c r="I4" t="n">
-        <v>11750.2123</v>
+        <v>11919.8706</v>
       </c>
     </row>
     <row r="5">
@@ -1384,13 +1384,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>658.5575727633415</v>
+        <v>1106.947020254855</v>
       </c>
       <c r="H5" t="n">
-        <v>11397.86744</v>
+        <v>12628.67994</v>
       </c>
       <c r="I5" t="n">
-        <v>10589.9866</v>
+        <v>11573.1087</v>
       </c>
     </row>
     <row r="6">
@@ -1417,13 +1417,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1379.497307325229</v>
+        <v>1637.142369517997</v>
       </c>
       <c r="H6" t="n">
-        <v>11842.4705</v>
+        <v>12216.30614</v>
       </c>
       <c r="I6" t="n">
-        <v>10372.1816</v>
+        <v>10390.432</v>
       </c>
     </row>
     <row r="7">
@@ -1450,13 +1450,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1027.965079479819</v>
+        <v>867.3822948542314</v>
       </c>
       <c r="H7" t="n">
-        <v>11769.86464</v>
+        <v>12641.17132</v>
       </c>
       <c r="I7" t="n">
-        <v>10556.5027</v>
+        <v>11655.1163</v>
       </c>
     </row>
   </sheetData>
@@ -1544,13 +1544,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>38.48591002682671</v>
+        <v>40.87643723742322</v>
       </c>
       <c r="H2" t="n">
-        <v>557.3783599999999</v>
+        <v>507.6675999999999</v>
       </c>
       <c r="I2" t="n">
-        <v>511.4851</v>
+        <v>472.4385</v>
       </c>
     </row>
     <row r="3">
@@ -1577,13 +1577,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>42.01442323119528</v>
+        <v>65.21131537385213</v>
       </c>
       <c r="H3" t="n">
-        <v>524.7442</v>
+        <v>468.2537600000001</v>
       </c>
       <c r="I3" t="n">
-        <v>472.8957</v>
+        <v>386.896</v>
       </c>
     </row>
     <row r="4">
@@ -1610,13 +1610,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>75.30412979382331</v>
+        <v>41.33860110935058</v>
       </c>
       <c r="H4" t="n">
-        <v>511.6427</v>
+        <v>552.9428399999999</v>
       </c>
       <c r="I4" t="n">
-        <v>418.0779</v>
+        <v>511.4706</v>
       </c>
     </row>
     <row r="5">
@@ -1643,13 +1643,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>31.35289231027987</v>
+        <v>46.52777561115509</v>
       </c>
       <c r="H5" t="n">
-        <v>570.1539</v>
+        <v>558.09998</v>
       </c>
       <c r="I5" t="n">
-        <v>523.0711</v>
+        <v>510.847</v>
       </c>
     </row>
     <row r="6">
@@ -1676,13 +1676,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>19.9121110559624</v>
+        <v>28.21055818453442</v>
       </c>
       <c r="H6" t="n">
-        <v>503.383</v>
+        <v>522.77266</v>
       </c>
       <c r="I6" t="n">
-        <v>484.7215</v>
+        <v>490.3805</v>
       </c>
     </row>
     <row r="7">
@@ -1709,13 +1709,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>72.92079524845413</v>
+        <v>61.38756317278772</v>
       </c>
       <c r="H7" t="n">
-        <v>497.11308</v>
+        <v>542.97506</v>
       </c>
       <c r="I7" t="n">
-        <v>409.8304</v>
+        <v>484.4864</v>
       </c>
     </row>
   </sheetData>
@@ -1803,13 +1803,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>25.65163246875333</v>
+        <v>25.89610202766045</v>
       </c>
       <c r="H2" t="n">
-        <v>260.79182</v>
+        <v>233.36342</v>
       </c>
       <c r="I2" t="n">
-        <v>217.0898</v>
+        <v>198.8525</v>
       </c>
     </row>
     <row r="3">
@@ -1836,13 +1836,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>61.75007856232251</v>
+        <v>63.49398550364436</v>
       </c>
       <c r="H3" t="n">
-        <v>243.89886</v>
+        <v>263.88612</v>
       </c>
       <c r="I3" t="n">
-        <v>186.6968</v>
+        <v>207.3536</v>
       </c>
     </row>
     <row r="4">
@@ -1869,13 +1869,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>36.60093839571606</v>
+        <v>22.85236975155978</v>
       </c>
       <c r="H4" t="n">
-        <v>230.41408</v>
+        <v>226.64798</v>
       </c>
       <c r="I4" t="n">
-        <v>183.2131</v>
+        <v>209.1884</v>
       </c>
     </row>
     <row r="5">
@@ -1902,13 +1902,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>28.40493065636675</v>
+        <v>38.1595477544874</v>
       </c>
       <c r="H5" t="n">
-        <v>219.00606</v>
+        <v>191.83258</v>
       </c>
       <c r="I5" t="n">
-        <v>185.0202</v>
+        <v>132.337</v>
       </c>
     </row>
     <row r="6">
@@ -1935,13 +1935,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>38.03248511190137</v>
+        <v>26.57540943330888</v>
       </c>
       <c r="H6" t="n">
-        <v>259.24188</v>
+        <v>234.69674</v>
       </c>
       <c r="I6" t="n">
-        <v>220.0491</v>
+        <v>205.4567</v>
       </c>
     </row>
     <row r="7">
@@ -1968,13 +1968,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>32.80071024386518</v>
+        <v>16.19556663185955</v>
       </c>
       <c r="H7" t="n">
-        <v>245.60972</v>
+        <v>235.92808</v>
       </c>
       <c r="I7" t="n">
-        <v>201.4534</v>
+        <v>209.0612</v>
       </c>
     </row>
   </sheetData>
@@ -2062,13 +2062,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>82139.86285949964</v>
+        <v>99425.41543711444</v>
       </c>
       <c r="H2" t="n">
-        <v>629259.4204599999</v>
+        <v>633729.06134</v>
       </c>
       <c r="I2" t="n">
-        <v>554317.7411</v>
+        <v>480832.4097</v>
       </c>
     </row>
     <row r="3">
@@ -2095,13 +2095,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>121418.3957055224</v>
+        <v>52818.14373243946</v>
       </c>
       <c r="H3" t="n">
-        <v>702065.5274199999</v>
+        <v>743464.65056</v>
       </c>
       <c r="I3" t="n">
-        <v>541985.6921</v>
+        <v>675409.7943</v>
       </c>
     </row>
     <row r="4">
@@ -2128,13 +2128,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>106731.9329697615</v>
+        <v>129150.6663096203</v>
       </c>
       <c r="H4" t="n">
-        <v>700773.1259600001</v>
+        <v>617044.5622400001</v>
       </c>
       <c r="I4" t="n">
-        <v>541985.3112999999</v>
+        <v>420118.3565</v>
       </c>
     </row>
     <row r="5">
@@ -2161,13 +2161,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>98225.18798888472</v>
+        <v>221867.6249859901</v>
       </c>
       <c r="H5" t="n">
-        <v>631785.22728</v>
+        <v>668533.86226</v>
       </c>
       <c r="I5" t="n">
-        <v>513340.3838</v>
+        <v>490862.3612</v>
       </c>
     </row>
     <row r="6">
@@ -2194,13 +2194,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>132192.844604341</v>
+        <v>86551.05731756629</v>
       </c>
       <c r="H6" t="n">
-        <v>612732.2150399999</v>
+        <v>676537.74808</v>
       </c>
       <c r="I6" t="n">
-        <v>439867.7337</v>
+        <v>532093.8329</v>
       </c>
     </row>
     <row r="7">
@@ -2227,13 +2227,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>163768.3818388118</v>
+        <v>84024.32754457422</v>
       </c>
       <c r="H7" t="n">
-        <v>589324.41606</v>
+        <v>662551.3906400001</v>
       </c>
       <c r="I7" t="n">
-        <v>363070.1459</v>
+        <v>538511.7928000001</v>
       </c>
     </row>
   </sheetData>
@@ -2321,13 +2321,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.4915766216979811</v>
+        <v>0.5971260687660521</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4557</v>
+        <v>0.69272</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0682</v>
+        <v>0.1839</v>
       </c>
     </row>
     <row r="3">
@@ -2354,13 +2354,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.1157866486258238</v>
+        <v>0.8458535168692036</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09386000000000001</v>
+        <v>0.68302</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0001</v>
+        <v>0.0046</v>
       </c>
     </row>
     <row r="4">
@@ -2387,13 +2387,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.37617080296057</v>
+        <v>0.2342844147612047</v>
       </c>
       <c r="H4" t="n">
-        <v>0.38564</v>
+        <v>0.2928799999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0104</v>
+        <v>0.0486</v>
       </c>
     </row>
     <row r="5">
@@ -2420,13 +2420,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0.4786788620776983</v>
+        <v>0.7047567573283707</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4325599999999999</v>
+        <v>0.68652</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0002</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="6">
@@ -2453,13 +2453,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0.1469804306702084</v>
+        <v>0.3872438095050715</v>
       </c>
       <c r="H6" t="n">
-        <v>0.11678</v>
+        <v>0.43524</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0002</v>
+        <v>0.0071</v>
       </c>
     </row>
     <row r="7">
@@ -2486,13 +2486,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.193724336687495</v>
+        <v>0.4489049710127969</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5771200000000001</v>
+        <v>0.38404</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0071</v>
+        <v>0.0081</v>
       </c>
     </row>
   </sheetData>
@@ -2580,13 +2580,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>165686656363.8342</v>
+        <v>99259477924.72134</v>
       </c>
       <c r="H2" t="n">
-        <v>249162070343.1857</v>
+        <v>117523181459.0076</v>
       </c>
       <c r="I2" t="n">
-        <v>32846362422.8336</v>
+        <v>3258581024.9093</v>
       </c>
     </row>
     <row r="3">
@@ -2613,13 +2613,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>186832167287.9125</v>
+        <v>130257738920.7657</v>
       </c>
       <c r="H3" t="n">
-        <v>282898446388.9989</v>
+        <v>212833133361.048</v>
       </c>
       <c r="I3" t="n">
-        <v>115520177463.9321</v>
+        <v>22301875699.1304</v>
       </c>
     </row>
     <row r="4">
@@ -2646,13 +2646,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>167588292337.2573</v>
+        <v>49780609578.71429</v>
       </c>
       <c r="H4" t="n">
-        <v>165833964950.5886</v>
+        <v>122589279656.7849</v>
       </c>
       <c r="I4" t="n">
-        <v>193804058.3181</v>
+        <v>48541632039.7682</v>
       </c>
     </row>
     <row r="5">
@@ -2679,13 +2679,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>102351560437.0998</v>
+        <v>129150725140.3167</v>
       </c>
       <c r="H5" t="n">
-        <v>89714950874.26392</v>
+        <v>107327363756.9536</v>
       </c>
       <c r="I5" t="n">
-        <v>1163319759.3532</v>
+        <v>12077815403.9756</v>
       </c>
     </row>
     <row r="6">
@@ -2712,13 +2712,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>14402991645.01629</v>
+        <v>102958172982.9337</v>
       </c>
       <c r="H6" t="n">
-        <v>43218733768.76717</v>
+        <v>116580862034.8071</v>
       </c>
       <c r="I6" t="n">
-        <v>21540801478.1638</v>
+        <v>6524159381.6133</v>
       </c>
     </row>
     <row r="7">
@@ -2745,13 +2745,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>118279676642.4362</v>
+        <v>78115976885.33308</v>
       </c>
       <c r="H7" t="n">
-        <v>130080663749.5233</v>
+        <v>68710646755.63744</v>
       </c>
       <c r="I7" t="n">
-        <v>1054228480.6476</v>
+        <v>2726514617.1257</v>
       </c>
     </row>
   </sheetData>
@@ -2839,13 +2839,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2645599436891380</v>
+        <v>955023623225895.8</v>
       </c>
       <c r="H2" t="n">
-        <v>1.026243613305946e+16</v>
+        <v>9861233160861486</v>
       </c>
       <c r="I2" t="n">
-        <v>7503690256960463</v>
+        <v>8729391134443771</v>
       </c>
     </row>
     <row r="3">
@@ -2872,13 +2872,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>690299044773312.2</v>
+        <v>3012134138115961</v>
       </c>
       <c r="H3" t="n">
-        <v>7912041706478312</v>
+        <v>9582163885512764</v>
       </c>
       <c r="I3" t="n">
-        <v>6723052033765725</v>
+        <v>6820086315159471</v>
       </c>
     </row>
     <row r="4">
@@ -2905,13 +2905,13 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1185533487639653</v>
+        <v>1504211702602553</v>
       </c>
       <c r="H4" t="n">
-        <v>9904278546515194</v>
+        <v>8514079842554832</v>
       </c>
       <c r="I4" t="n">
-        <v>8020158440189516</v>
+        <v>6086606790638312</v>
       </c>
     </row>
     <row r="5">
@@ -2938,13 +2938,13 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2284593194148946</v>
+        <v>3164412425455727</v>
       </c>
       <c r="H5" t="n">
-        <v>8788374392489395</v>
+        <v>1.124393830850122e+16</v>
       </c>
       <c r="I5" t="n">
-        <v>5846489318111023</v>
+        <v>7580086636739949</v>
       </c>
     </row>
     <row r="6">
@@ -2971,13 +2971,13 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>3302704102680068</v>
+        <v>1477010380859709</v>
       </c>
       <c r="H6" t="n">
-        <v>1.057886098143331e+16</v>
+        <v>8575000436035427</v>
       </c>
       <c r="I6" t="n">
-        <v>7124640035859497</v>
+        <v>7009619868328849</v>
       </c>
     </row>
     <row r="7">
@@ -3004,13 +3004,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2643338526076318</v>
+        <v>2592002394454354</v>
       </c>
       <c r="H7" t="n">
-        <v>1.068149935920339e+16</v>
+        <v>1.060069548523129e+16</v>
       </c>
       <c r="I7" t="n">
-        <v>8477101498776278</v>
+        <v>7338958942283823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>